<commit_message>
Agregue la interfaz y el metodo para agregar usuario
</commit_message>
<xml_diff>
--- a/Informacion_Empleados.xlsx
+++ b/Informacion_Empleados.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>Lucia</t>
   </si>
@@ -168,6 +168,24 @@
   </si>
   <si>
     <t>Rojas</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Puesto</t>
+  </si>
+  <si>
+    <t>Sueldo Mensual</t>
+  </si>
+  <si>
+    <t>Fecha de Ingreso</t>
+  </si>
+  <si>
+    <t>Numero de Nomina</t>
   </si>
 </sst>
 </file>
@@ -209,9 +227,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,415 +508,457 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>13000</v>
-      </c>
-      <c r="E1" s="1">
-        <v>42889</v>
-      </c>
-      <c r="F1">
-        <v>43230001</v>
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>13000</v>
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>15000</v>
       </c>
       <c r="E2" s="1">
-        <v>42890</v>
+        <v>42889</v>
       </c>
       <c r="F2">
-        <v>43230002</v>
+        <v>2343001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>13000</v>
+        <v>5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>16000</v>
       </c>
       <c r="E3" s="1">
-        <v>42891</v>
+        <v>42890</v>
       </c>
       <c r="F3">
-        <v>43230003</v>
+        <f>F2+1</f>
+        <v>2343002</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
         <v>13000</v>
       </c>
       <c r="E4" s="1">
-        <v>42892</v>
+        <v>42891</v>
       </c>
       <c r="F4">
-        <v>43230004</v>
+        <f t="shared" ref="F4:F21" si="0">F3+1</f>
+        <v>2343003</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2">
         <v>13000</v>
       </c>
       <c r="E5" s="1">
-        <v>42893</v>
+        <v>42892</v>
       </c>
       <c r="F5">
-        <v>43230005</v>
+        <f t="shared" si="0"/>
+        <v>2343004</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2">
         <v>13000</v>
       </c>
       <c r="E6" s="1">
-        <v>42894</v>
+        <v>42893</v>
       </c>
       <c r="F6">
-        <v>43230006</v>
+        <f t="shared" si="0"/>
+        <v>2343005</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2">
         <v>13000</v>
       </c>
       <c r="E7" s="1">
-        <v>42895</v>
+        <v>42894</v>
       </c>
       <c r="F7">
-        <v>43230007</v>
+        <f t="shared" si="0"/>
+        <v>2343006</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2">
         <v>13000</v>
       </c>
       <c r="E8" s="1">
-        <v>42896</v>
+        <v>42895</v>
       </c>
       <c r="F8">
-        <v>43230008</v>
+        <f t="shared" si="0"/>
+        <v>2343007</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
         <v>13000</v>
       </c>
       <c r="E9" s="1">
-        <v>42897</v>
+        <v>42896</v>
       </c>
       <c r="F9">
-        <v>43230009</v>
+        <f t="shared" si="0"/>
+        <v>2343008</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2">
         <v>13000</v>
       </c>
       <c r="E10" s="1">
-        <v>42898</v>
+        <v>42897</v>
       </c>
       <c r="F10">
-        <v>43230010</v>
+        <f t="shared" si="0"/>
+        <v>2343009</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>13000</v>
       </c>
       <c r="E11" s="1">
-        <v>42899</v>
+        <v>42898</v>
       </c>
       <c r="F11">
-        <v>43230011</v>
+        <f t="shared" si="0"/>
+        <v>2343010</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2">
         <v>13000</v>
       </c>
       <c r="E12" s="1">
-        <v>42900</v>
+        <v>42899</v>
       </c>
       <c r="F12">
-        <v>43230012</v>
+        <f t="shared" si="0"/>
+        <v>2343011</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>13000</v>
       </c>
       <c r="E13" s="1">
-        <v>42901</v>
+        <v>42900</v>
       </c>
       <c r="F13">
-        <v>43230013</v>
+        <f t="shared" si="0"/>
+        <v>2343012</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>13000</v>
       </c>
       <c r="E14" s="1">
-        <v>42902</v>
+        <v>42901</v>
       </c>
       <c r="F14">
-        <v>43230014</v>
+        <f t="shared" si="0"/>
+        <v>2343013</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>13000</v>
       </c>
       <c r="E15" s="1">
-        <v>42903</v>
+        <v>42902</v>
       </c>
       <c r="F15">
-        <v>43230015</v>
+        <f t="shared" si="0"/>
+        <v>2343014</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>13000</v>
       </c>
       <c r="E16" s="1">
-        <v>42904</v>
+        <v>42903</v>
       </c>
       <c r="F16">
-        <v>43230016</v>
+        <f t="shared" si="0"/>
+        <v>2343015</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2">
         <v>13000</v>
       </c>
       <c r="E17" s="1">
-        <v>42905</v>
+        <v>42904</v>
       </c>
       <c r="F17">
-        <v>43230017</v>
+        <f t="shared" si="0"/>
+        <v>2343016</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18">
+        <v>18</v>
+      </c>
+      <c r="D18" s="2">
         <v>13000</v>
       </c>
       <c r="E18" s="1">
-        <v>42906</v>
+        <v>42905</v>
       </c>
       <c r="F18">
-        <v>43230018</v>
+        <f t="shared" si="0"/>
+        <v>2343017</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>42</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>13000</v>
       </c>
       <c r="E19" s="1">
-        <v>42907</v>
+        <v>42906</v>
       </c>
       <c r="F19">
-        <v>43230019</v>
+        <f t="shared" si="0"/>
+        <v>2343018</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="2">
+        <v>13000</v>
+      </c>
+      <c r="E20" s="1">
+        <v>42907</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>2343019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>45</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>46</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="D20">
-        <v>13000</v>
-      </c>
-      <c r="E20" s="1">
+      <c r="D21" s="2">
+        <v>13000</v>
+      </c>
+      <c r="E21" s="1">
         <v>42908</v>
       </c>
-      <c r="F20">
-        <v>43230020</v>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>2343020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>